<commit_message>
Unlocked a cell needed by user
</commit_message>
<xml_diff>
--- a/templates/NOMADS_PCR_Worksheet.xlsx
+++ b/templates/NOMADS_PCR_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025" codeName="{372AB895-14C1-FC20-EB20-F1B4BCFD95AE}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956B2F9A-9328-4B07-B4A9-F9FED3EE643B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952FA0BF-956B-48F8-A4A4-E25D95611892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29625" activeTab="4" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" activeTab="4" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -23,20 +23,21 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Instructions!#REF!</definedName>
-    <definedName name="exp_assay">Assay!$D$11</definedName>
-    <definedName name="exp_date">Assay!$D$2</definedName>
-    <definedName name="exp_id">Assay!$D$5</definedName>
-    <definedName name="exp_notes">Assay!$D$17</definedName>
-    <definedName name="exp_rxns">Assay!$D$16</definedName>
-    <definedName name="exp_summary">Assay!$D$9</definedName>
+    <definedName name="exp_assay">Assay!$C$11</definedName>
+    <definedName name="exp_date">Assay!$C$2</definedName>
+    <definedName name="exp_id">Assay!$C$5</definedName>
+    <definedName name="exp_notes">Assay!$C$17</definedName>
+    <definedName name="exp_rxns">Assay!$C$16</definedName>
+    <definedName name="exp_summary">Assay!$C$9</definedName>
     <definedName name="exp_type">reference!$B$6</definedName>
-    <definedName name="exp_user">Assay!$D$3</definedName>
+    <definedName name="exp_user">Assay!$C$3</definedName>
     <definedName name="exp_version">reference!$B$7</definedName>
     <definedName name="pcr_dna_source">Assay!#REF!</definedName>
-    <definedName name="pcr_enzyme">Assay!$D$15</definedName>
-    <definedName name="pcr_primers">Assay!$D$13</definedName>
-    <definedName name="pcr_primersource">Assay!$D$14</definedName>
-    <definedName name="pcr_targetpanel">Assay!$D$12</definedName>
+    <definedName name="pcr_enzyme">Assay!$C$15</definedName>
+    <definedName name="pcr_primers">Assay!$C$13</definedName>
+    <definedName name="pcr_primersource">Assay!$C$14</definedName>
+    <definedName name="pcr_targetpanel">Assay!$C$12</definedName>
+    <definedName name="template_vol">Assay!$D$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="284">
   <si>
     <t>Assumptions</t>
   </si>
@@ -1141,12 +1142,6 @@
     <t>Q5</t>
   </si>
   <si>
-    <t>30 sec</t>
-  </si>
-  <si>
-    <t>7 sec</t>
-  </si>
-  <si>
     <t>KAPA HiFi ReadyMix</t>
   </si>
   <si>
@@ -1183,9 +1178,6 @@
     <t>sample_type</t>
   </si>
   <si>
-    <t>Added sample type</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
@@ -1193,6 +1185,30 @@
   </si>
   <si>
     <t>Negative</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>x35</t>
+  </si>
+  <si>
+    <t>NOMADS8 and 16</t>
+  </si>
+  <si>
+    <t>Corrections to volumes</t>
+  </si>
+  <si>
+    <t>Selected Primer Set</t>
+  </si>
+  <si>
+    <t>template_vol</t>
+  </si>
+  <si>
+    <t>Selected polymerase</t>
+  </si>
+  <si>
+    <t>KAPA HiFI ReadyMix (2x)</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1502,15 +1518,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1521,15 +1528,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1632,7 +1630,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1672,20 +1670,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1703,7 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1743,7 +1741,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1751,23 +1749,23 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1777,21 +1775,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1827,21 +1825,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1849,57 +1842,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1924,35 +1880,69 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1960,7 +1950,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1974,7 +1968,72 @@
     <cellStyle name="Normal 4" xfId="3" xr:uid="{50147B5D-B577-4D84-8D3E-2790725A5EE2}"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2360,34 +2419,6 @@
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2402,24 +2433,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C103716-E393-43AA-872A-215BD28108E4}" name="tbl_PCR" displayName="tbl_PCR" ref="A2:K98" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C103716-E393-43AA-872A-215BD28108E4}" name="tbl_PCR" displayName="tbl_PCR" ref="A2:K98" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="A2:K98" xr:uid="{4C103716-E393-43AA-872A-215BD28108E4}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{AFEE5217-53A1-450F-B6A8-E87D945E0FAE}" name="#" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{0CF8190A-662E-422B-8BDD-34F3D27B34F2}" name="Well" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{CE61E1E1-E9B3-4D58-9DFE-1AB6DDFCD05A}" name="Sample ID" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{9795EF0E-2DE1-455A-A3FF-0804F7CBA8C3}" name="Extraction ID" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{BC0F75E0-A79C-490C-9405-CD6FA4A793F8}" name="Sample Type" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA identifier" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{59846CDB-FD66-45CD-A212-013D460992B1}" name="PCR Identifier" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{AFEE5217-53A1-450F-B6A8-E87D945E0FAE}" name="#" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{0CF8190A-662E-422B-8BDD-34F3D27B34F2}" name="Well" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{CE61E1E1-E9B3-4D58-9DFE-1AB6DDFCD05A}" name="Sample ID" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{9795EF0E-2DE1-455A-A3FF-0804F7CBA8C3}" name="Extraction ID" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{BC0F75E0-A79C-490C-9405-CD6FA4A793F8}" name="Sample Type" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{B3E809FC-AA96-4329-8BC3-6D3188F7C694}" name="sWGA identifier" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{59846CDB-FD66-45CD-A212-013D460992B1}" name="PCR Identifier" dataDxfId="25">
       <calculatedColumnFormula>IF(LEN(tbl_PCR[[#This Row],[sWGA identifier]])=0,"",CONCATENATE(exp_id,"_",tbl_PCR[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{734522B3-E102-4EBF-AD04-14C3F7B67107}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{D2BFD013-75EF-450B-A4E3-95DAB8A07EC6}" name="PCR Dilution Factor" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{96ADB29E-A594-4912-850A-45B8B3904B4D}" name="PCR [DNA] (ng / µl)" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{734522B3-E102-4EBF-AD04-14C3F7B67107}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{D2BFD013-75EF-450B-A4E3-95DAB8A07EC6}" name="PCR Dilution Factor" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{96ADB29E-A594-4912-850A-45B8B3904B4D}" name="PCR [DNA] (ng / µl)" dataDxfId="22">
       <calculatedColumnFormula>IF(OR(H3="",I3=""),"",SUM(H3*I3))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{87CC627F-41F3-42EC-BA06-893DB14E3545}" name="Proceed with library prep" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{87CC627F-41F3-42EC-BA06-893DB14E3545}" name="Proceed with library prep" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2437,21 +2468,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}" name="tbl_Assays" displayName="tbl_Assays" ref="E2:G8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}" name="tbl_Assays" displayName="tbl_Assays" ref="E2:G8" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="E2:G8" xr:uid="{488B678F-87F5-452A-9808-8C26D87C6316}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{981BF5AE-121F-4AF8-855F-49DE509E86E1}" name="Assay Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{AECC9098-A69C-44D7-87A5-086086FD999D}" name="Targets" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{20A98561-A069-41FD-A7B3-766B6336516C}" name="Primer Set" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{981BF5AE-121F-4AF8-855F-49DE509E86E1}" name="Assay Name" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{AECC9098-A69C-44D7-87A5-086086FD999D}" name="Targets" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{20A98561-A069-41FD-A7B3-766B6336516C}" name="Primer Set" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F7724E8-27D2-44E9-85B4-57378D47D280}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{1F7724E8-27D2-44E9-85B4-57378D47D280}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F7724E8-27D2-44E9-85B4-57378D47D280}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:N2" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{1F7724E8-27D2-44E9-85B4-57378D47D280}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{CF92ACF9-25F8-4BAA-B9F1-567A722EDD10}" name="expt_id">
       <calculatedColumnFormula>IF(LEN(exp_id)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
@@ -2488,6 +2519,9 @@
     <tableColumn id="9" xr3:uid="{5C17D014-189E-43E2-A899-4574390B7A58}" name="pcr_targetpanel">
       <calculatedColumnFormula>IF(LEN(pcr_targetpanel)=0,"",pcr_targetpanel)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="14" xr3:uid="{B1248788-8BBB-4F40-90D1-7B509917F807}" name="template_vol">
+      <calculatedColumnFormula>IF(LEN(template_vol)=0,"",template_vol)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="13" xr3:uid="{4786D324-56A9-420B-A7CB-8083E29E50BD}" name="pcr_enzyme">
       <calculatedColumnFormula>IF(pcr_enzyme=0,"",pcr_enzyme)</calculatedColumnFormula>
     </tableColumn>
@@ -2500,22 +2534,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DBBF945E-5383-4B75-AC55-E268322A374B}" name="tbl_rxn_metadata" displayName="tbl_rxn_metadata" ref="A1:G97" totalsRowShown="0">
   <autoFilter ref="A1:G97" xr:uid="{DBBF945E-5383-4B75-AC55-E268322A374B}"/>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{1282264C-DD99-4BA3-8DB8-0E9363F6BA7C}" name="sample_id" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{1282264C-DD99-4BA3-8DB8-0E9363F6BA7C}" name="sample_id" dataDxfId="15">
       <calculatedColumnFormula>IF(LEN(PCR!C3),PCR!C3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3FFBD26A-1339-451E-AF0C-51A92B0387C9}" name="extraction_id" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{3FFBD26A-1339-451E-AF0C-51A92B0387C9}" name="extraction_id" dataDxfId="14">
       <calculatedColumnFormula>IF(LEN(PCR!D3),PCR!D3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AE08A273-A276-4DC2-A55C-31491BBF4293}" name="sample_type" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{AE08A273-A276-4DC2-A55C-31491BBF4293}" name="sample_type" dataDxfId="13">
       <calculatedColumnFormula>IF(LEN(PCR!E3),PCR!E3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5545E98D-0544-4375-81E6-330418C07C1D}" name="expt_id" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{5545E98D-0544-4375-81E6-330418C07C1D}" name="expt_id" dataDxfId="12">
       <calculatedColumnFormula>IF(LEN(PCR!F3)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA58F3D6-4DB3-46FB-B1A4-0E7CBCBBBC84}" name="swga_identifier" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{EA58F3D6-4DB3-46FB-B1A4-0E7CBCBBBC84}" name="swga_identifier" dataDxfId="11">
       <calculatedColumnFormula>IF(LEN(PCR!F3),PCR!F3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{0E0D5C67-8A41-4FE0-9D6C-4C0D6A331B2E}" name="pcr_identifier" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{0E0D5C67-8A41-4FE0-9D6C-4C0D6A331B2E}" name="pcr_identifier" dataDxfId="10">
       <calculatedColumnFormula>IF(LEN(PCR!G3),PCR!G3,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{4845F373-7505-41AE-BC4F-278230D9F085}" name="pcr_product_ngul">
@@ -2827,1563 +2861,1193 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5" hidden="1" customWidth="1"/>
-    <col min="2" max="9" width="9" style="7" customWidth="1"/>
+    <col min="1" max="8" width="9" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="94" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-    </row>
-    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="95" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="I2" s="95"/>
-      <c r="L2" s="91" t="s">
+      <c r="H2" s="82"/>
+      <c r="K2" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="M2" s="91"/>
-    </row>
-    <row r="3" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="L2" s="89"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" t="s">
         <v>156</v>
       </c>
-      <c r="L3" s="89" t="s">
+      <c r="K3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="89"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="75" t="s">
+      <c r="L3" s="95"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="25" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="K4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="90"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="s">
+      <c r="L4" s="96"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="99" t="str">
-        <f>IF(OR(ISBLANK(D3),ISBLANK(D4)),"",CONCATENATE("PC",VLOOKUP(D3,reference!I3:J8,2,FALSE),D4))</f>
-        <v/>
-      </c>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="15" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="86" t="str">
+        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("PC",VLOOKUP(C3,reference!I3:J8,2,FALSE),C4))</f>
+        <v/>
+      </c>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="92" t="s">
+      <c r="K5" s="98" t="s">
         <v>199</v>
       </c>
-      <c r="M5" s="92"/>
-    </row>
-    <row r="6" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73" t="s">
+      <c r="L5" s="98"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="100" t="str">
-        <f>IF(OR(ISBLANK(D2),ISBLANK(D3),LEN(D5)=0),"",CONCATENATE(D2,"_PCR_",D5))</f>
-        <v/>
-      </c>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="22"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-    </row>
-    <row r="7" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="103" t="s">
+      <c r="B6" s="83"/>
+      <c r="C6" s="87" t="str">
+        <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_PCR_",C5))</f>
+        <v/>
+      </c>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="22"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="103" t="s">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" t="s">
+      <c r="B8" s="78"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="104" t="s">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="102" t="str">
-        <f>IF(OR(LEN(D7)=0, LEN(D8)=0),"",CONCATENATE(D7,"_Batch",D8))</f>
-        <v/>
-      </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="15" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="99" t="str">
+        <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
+        <v/>
+      </c>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="104" t="s">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
         <v>205</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="105" t="str">
-        <f>IF(OR(LEN(D6)=0,LEN(exp_summary)=0),"",CONCATENATE(D6,"_",exp_summary,".xlsx"))</f>
-        <v/>
-      </c>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="75" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80" t="str">
+        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary,".xlsx"))</f>
+        <v/>
+      </c>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" t="s">
+      <c r="B11" s="75"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="73" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="72" t="str">
-        <f>IF(ISBLANK(D11),"",VLOOKUP(D11,tbl_Assays[],2,FALSE))</f>
-        <v/>
-      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72" t="str">
+        <f>IF(ISBLANK(C11),"",VLOOKUP(C11,tbl_Assays[],2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="D12" s="72"/>
       <c r="E12" s="72"/>
       <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="15" t="s">
+      <c r="G12" s="15" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="73" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="72" t="str">
-        <f>IF(ISBLANK(D11),"",VLOOKUP(D11,tbl_Assays[],3,FALSE))</f>
-        <v/>
-      </c>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72" t="str">
+        <f>IF(ISBLANK(C11),"",VLOOKUP(C11,tbl_Assays[],3,FALSE))</f>
+        <v/>
+      </c>
+      <c r="D13" s="72"/>
       <c r="E13" s="72"/>
       <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="75" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="15" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="15" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="75" t="s">
-        <v>265</v>
-      </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="75" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+      <c r="B16" s="75"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="G19"/>
       <c r="H19"/>
-      <c r="I19"/>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="60" t="s">
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="63">
+      <c r="D20" s="63">
         <v>0.1</v>
       </c>
+      <c r="E20" s="64"/>
       <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-    </row>
-    <row r="21" spans="1:14" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B21" s="79" t="s">
+    </row>
+    <row r="21" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80" t="str">
+      <c r="E21" s="76"/>
+      <c r="F21" s="76" t="str">
         <f>CONCATENATE("MM x",exp_rxns, " (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="H21" s="80"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="83" t="s">
+      <c r="G21" s="76"/>
+      <c r="H21" s="8"/>
+      <c r="J21" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="83"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="65" t="s">
+        <v>14</v>
+      </c>
       <c r="M21" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="N21" s="65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B22" s="81" t="s">
-        <v>217</v>
-      </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="78">
+    <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="90" t="str">
+        <f>reference!E24</f>
+        <v/>
+      </c>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="101"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="91" t="str">
+        <f>reference!E56</f>
+        <v/>
+      </c>
+      <c r="K22" s="91"/>
+      <c r="L22" s="67" t="str">
+        <f>reference!F56</f>
+        <v/>
+      </c>
+      <c r="M22" s="67" t="str">
+        <f>reference!G56</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="90" t="str">
+        <f>reference!E25</f>
+        <v/>
+      </c>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="94" t="str">
+        <f>reference!F25</f>
+        <v/>
+      </c>
+      <c r="E23" s="94"/>
+      <c r="F23" s="97" t="str">
+        <f>IFERROR(SUM(D23*exp_rxns*(1+$D$20)),"")</f>
+        <v/>
+      </c>
+      <c r="G23" s="97"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="91" t="str">
+        <f>reference!E57</f>
+        <v/>
+      </c>
+      <c r="K23" s="91"/>
+      <c r="L23" s="67" t="str">
+        <f>reference!F57</f>
+        <v/>
+      </c>
+      <c r="M23" s="67" t="str">
+        <f>reference!G57</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="90" t="str">
+        <f>reference!E26</f>
+        <v/>
+      </c>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="94" t="str">
+        <f>reference!F26</f>
+        <v/>
+      </c>
+      <c r="E24" s="94"/>
+      <c r="F24" s="97" t="str">
+        <f>IFERROR(SUM(D24*exp_rxns*(1+$D$20)),"")</f>
+        <v/>
+      </c>
+      <c r="G24" s="97"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="91" t="str">
+        <f>reference!E58</f>
+        <v/>
+      </c>
+      <c r="K24" s="91"/>
+      <c r="L24" s="67" t="str">
+        <f>reference!F58</f>
+        <v/>
+      </c>
+      <c r="M24" s="67" t="str">
+        <f>reference!G58</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="90" t="str">
+        <f>reference!E27</f>
+        <v/>
+      </c>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="94" t="str">
+        <f>reference!F27</f>
+        <v/>
+      </c>
+      <c r="E25" s="94"/>
+      <c r="F25" s="97" t="str">
+        <f>IFERROR(SUM(D25*exp_rxns*(1+$D$20)),"")</f>
+        <v/>
+      </c>
+      <c r="G25" s="97"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="91" t="str">
+        <f>reference!E59</f>
+        <v/>
+      </c>
+      <c r="K25" s="91"/>
+      <c r="L25" s="67" t="str">
+        <f>reference!F59</f>
+        <v/>
+      </c>
+      <c r="M25" s="67" t="str">
+        <f>reference!G59</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="90" t="str">
+        <f>reference!E28</f>
+        <v/>
+      </c>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="94" t="str">
+        <f>reference!F28</f>
+        <v/>
+      </c>
+      <c r="E26" s="94"/>
+      <c r="F26" s="97" t="str">
+        <f>IFERROR(SUM(D26*exp_rxns*(1+$D$20)),"")</f>
+        <v/>
+      </c>
+      <c r="G26" s="97"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="91" t="str">
+        <f>reference!E60</f>
+        <v/>
+      </c>
+      <c r="K26" s="91"/>
+      <c r="L26" s="67" t="str">
+        <f>reference!F60</f>
+        <v/>
+      </c>
+      <c r="M26" s="67" t="str">
+        <f>reference!G60</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="90" t="str">
+        <f>reference!E29</f>
+        <v/>
+      </c>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="94" t="str">
+        <f>reference!F29</f>
+        <v/>
+      </c>
+      <c r="E27" s="94"/>
+      <c r="F27" s="97" t="str">
+        <f>IFERROR(SUM(D27*exp_rxns*(1+$D$20)),"")</f>
+        <v/>
+      </c>
+      <c r="G27" s="97"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="102">
+        <f>SUM(D22:D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="102"/>
+      <c r="F28" s="69" t="str">
+        <f>CONCATENATE("Add ",SUM(D23:D27)," µl of MM to each well")</f>
+        <v>Add 0 µl of MM to each well</v>
+      </c>
+      <c r="G28" s="67"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="K30" s="103" t="s">
+        <v>163</v>
+      </c>
+      <c r="L30" s="103"/>
+      <c r="M30" s="103"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="8"/>
+      <c r="K32" s="104" t="s">
+        <v>164</v>
+      </c>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35" s="27">
         <v>1</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="82" t="s">
+      <c r="C35" s="27">
+        <v>2</v>
+      </c>
+      <c r="D35" s="27">
+        <v>3</v>
+      </c>
+      <c r="E35" s="27">
+        <v>4</v>
+      </c>
+      <c r="F35" s="27">
+        <v>5</v>
+      </c>
+      <c r="G35" s="27">
+        <v>6</v>
+      </c>
+      <c r="H35" s="27">
+        <v>7</v>
+      </c>
+      <c r="I35" s="27">
+        <v>8</v>
+      </c>
+      <c r="J35" s="27">
         <v>9</v>
       </c>
-      <c r="H22" s="82"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="86">
-        <v>93</v>
-      </c>
-      <c r="L22" s="86"/>
-      <c r="M22" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="N22" s="67"/>
-    </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B23" s="77" t="s">
-        <v>259</v>
-      </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="78">
-        <v>0.3</v>
-      </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="71">
-        <f>SUM(E23*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="71"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="84">
-        <v>98</v>
-      </c>
-      <c r="L23" s="84"/>
-      <c r="M23" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23" s="85" t="s">
+      <c r="K35" s="27">
+        <v>10</v>
+      </c>
+      <c r="L35" s="27">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B24" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="78">
-        <v>2</v>
-      </c>
-      <c r="F24" s="78"/>
-      <c r="G24" s="71">
-        <f>IF(E24=0,"",SUM(E24*exp_rxns*(1+$E$20)))</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="71"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="78">
-        <v>50</v>
-      </c>
-      <c r="L24" s="78"/>
-      <c r="M24" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" s="85"/>
-    </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B25" s="77" t="s">
-        <v>219</v>
-      </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78">
-        <v>5</v>
-      </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="71">
-        <f>IF(E25=0,"",SUM(E25*exp_rxns*(1+$E$20)))</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="71"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="81">
-        <v>60</v>
-      </c>
-      <c r="L25" s="81"/>
-      <c r="M25" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="N25" s="85"/>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B26" s="77" t="s">
+      <c r="M35" s="27">
         <v>12</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78">
-        <v>1.5</v>
-      </c>
-      <c r="F26" s="78"/>
-      <c r="G26" s="71">
-        <f>IF(E26=0,"",SUM(E26*exp_rxns*(1+$E$20)))</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="71"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="78">
-        <v>60</v>
-      </c>
-      <c r="L26" s="78"/>
-      <c r="M26" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="67"/>
-    </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="B27" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77">
-        <v>15.2</v>
-      </c>
-      <c r="F27" s="77"/>
-      <c r="G27" s="71">
-        <f>SUM(E27*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="71"/>
-      <c r="I27" s="8"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="78"/>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f>reference!$E$14</f>
-        <v>KAPA HiFi</v>
-      </c>
-      <c r="E28" s="74">
-        <f>SUM(E22:E27)</f>
-        <v>25</v>
-      </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="69" t="str">
-        <f>CONCATENATE("Add ",SUM(E23:E27)," µl of MM to each well")</f>
-        <v>Add 24 µl of MM to each well</v>
-      </c>
-      <c r="H28" s="67"/>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:14" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="B29" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80" t="str">
-        <f>CONCATENATE("MM x",exp_rxns, " (µl)")</f>
-        <v>MM x (µl)</v>
-      </c>
-      <c r="H29" s="80"/>
-      <c r="I29" s="8"/>
-      <c r="K29" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="L29" s="83"/>
-      <c r="M29" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="N29" s="65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="B30" s="81" t="s">
-        <v>217</v>
-      </c>
-      <c r="C30" s="81"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="78">
-        <v>1</v>
-      </c>
-      <c r="F30" s="78"/>
-      <c r="G30" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="82"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="86">
-        <v>93</v>
-      </c>
-      <c r="L30" s="86"/>
-      <c r="M30" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="N30" s="67"/>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="B31" s="77" t="s">
-        <v>264</v>
-      </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="78">
-        <v>12.5</v>
-      </c>
-      <c r="F31" s="78"/>
-      <c r="G31" s="71">
-        <f>SUM(E31*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="71"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="84">
-        <v>98</v>
-      </c>
-      <c r="L31" s="84"/>
-      <c r="M31" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="85" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="B32" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="78">
-        <v>1.5</v>
-      </c>
-      <c r="F32" s="78"/>
-      <c r="G32" s="71">
-        <f>IF(E32=0,"",SUM(E32*exp_rxns*(1+$E$20)))</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="71"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="78">
-        <v>50</v>
-      </c>
-      <c r="L32" s="78"/>
-      <c r="M32" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" s="85"/>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77">
-        <f>25-SUM(E30:F32)</f>
-        <v>10</v>
-      </c>
-      <c r="F33" s="77"/>
-      <c r="G33" s="71">
-        <f>SUM(E33*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="71"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="81">
-        <v>60</v>
-      </c>
-      <c r="L33" s="81"/>
-      <c r="M33" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="N33" s="85"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
-        <f>reference!$E$15</f>
-        <v>KAPA HiFi ReadyMix</v>
-      </c>
-      <c r="E34" s="74">
-        <f>SUM(E30:F33)</f>
-        <v>25</v>
-      </c>
-      <c r="F34" s="74"/>
-      <c r="G34" s="69" t="str">
-        <f>CONCATENATE("Add ",SUM(E31:E33)," µl of MM to each well")</f>
-        <v>Add 24 µl of MM to each well</v>
-      </c>
-      <c r="H34" s="67"/>
-      <c r="I34" s="66"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="78">
-        <v>60</v>
-      </c>
-      <c r="L34" s="78"/>
-      <c r="M34" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="N34" s="67"/>
-    </row>
-    <row r="35" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="B35" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80" t="str">
-        <f>CONCATENATE("MM x",exp_rxns, " (µl)")</f>
-        <v>MM x (µl)</v>
-      </c>
-      <c r="H35" s="80"/>
-      <c r="I35" s="8"/>
-      <c r="K35" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="L35" s="83"/>
-      <c r="M35" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="B36" s="81" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="78">
-        <v>8</v>
-      </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="82"/>
-      <c r="I36" s="8"/>
-      <c r="K36" s="86">
-        <v>98</v>
-      </c>
-      <c r="L36" s="86"/>
-      <c r="M36" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="N36" s="67"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="B37" s="77" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="78">
-        <v>14.5</v>
-      </c>
-      <c r="F37" s="78"/>
-      <c r="G37" s="71">
-        <f>SUM(E37*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="71"/>
-      <c r="I37" s="8"/>
-      <c r="K37" s="84">
-        <v>98</v>
-      </c>
-      <c r="L37" s="84"/>
-      <c r="M37" s="67" t="s">
-        <v>261</v>
-      </c>
-      <c r="N37" s="85" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="B38" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="78">
-        <v>2.5</v>
-      </c>
-      <c r="F38" s="78"/>
-      <c r="G38" s="71">
-        <f>IF(E38=0,"",SUM(E38*exp_rxns*(1+$E$20)))</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="71"/>
-      <c r="I38" s="8"/>
-      <c r="K38" s="78">
-        <v>98</v>
-      </c>
-      <c r="L38" s="78"/>
-      <c r="M38" s="67" t="s">
-        <v>262</v>
-      </c>
-      <c r="N38" s="85"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="B39" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77">
-        <f>SUM(25-SUM(E36:F38))</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="77"/>
-      <c r="G39" s="71">
-        <f>SUM(E39*exp_rxns*(1+$E$20))</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="71"/>
-      <c r="I39" s="8"/>
-      <c r="K39" s="81">
-        <v>64</v>
-      </c>
-      <c r="L39" s="81"/>
-      <c r="M39" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="N39" s="85"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
-        <f>reference!$E$16</f>
-        <v>Q5</v>
-      </c>
-      <c r="E40" s="74">
-        <f>SUM(E36:E39)</f>
-        <v>25</v>
-      </c>
-      <c r="F40" s="74"/>
-      <c r="G40" s="69" t="str">
-        <f>CONCATENATE("Add ",SUM(E37:E39)," µl of MM to each well")</f>
-        <v>Add 17 µl of MM to each well</v>
-      </c>
-      <c r="H40" s="67"/>
-      <c r="I40" s="8"/>
-      <c r="K40" s="78">
-        <v>64</v>
-      </c>
-      <c r="L40" s="78"/>
-      <c r="M40" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="N40" s="67"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="8"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="L42" s="87" t="s">
-        <v>163</v>
-      </c>
-      <c r="M42" s="87"/>
-      <c r="N42" s="87"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="95"/>
-      <c r="G43" s="95"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="8"/>
-      <c r="L44" s="88" t="s">
-        <v>164</v>
-      </c>
-      <c r="M44" s="88"/>
-      <c r="N44" s="88"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47"/>
-      <c r="C47" s="27">
-        <v>1</v>
-      </c>
-      <c r="D47" s="27">
-        <v>2</v>
-      </c>
-      <c r="E47" s="27">
-        <v>3</v>
-      </c>
-      <c r="F47" s="27">
-        <v>4</v>
-      </c>
-      <c r="G47" s="27">
-        <v>5</v>
-      </c>
-      <c r="H47" s="27">
-        <v>6</v>
-      </c>
-      <c r="I47" s="27">
-        <v>7</v>
-      </c>
-      <c r="J47" s="27">
-        <v>8</v>
-      </c>
-      <c r="K47" s="27">
-        <v>9</v>
-      </c>
-      <c r="L47" s="27">
-        <v>10</v>
-      </c>
-      <c r="M47" s="27">
-        <v>11</v>
-      </c>
-      <c r="N47" s="27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="28" t="s">
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="26" t="str">
+      <c r="B36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D3), "",PCR!D3)</f>
         <v/>
       </c>
-      <c r="D48" s="26" t="str">
+      <c r="C36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D11), "",PCR!D11)</f>
         <v/>
       </c>
-      <c r="E48" s="26" t="str">
+      <c r="D36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D19), "",PCR!D19)</f>
         <v/>
       </c>
-      <c r="F48" s="26" t="str">
+      <c r="E36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D27), "",PCR!D27)</f>
         <v/>
       </c>
-      <c r="G48" s="26" t="str">
+      <c r="F36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D35), "",PCR!D35)</f>
         <v/>
       </c>
-      <c r="H48" s="26" t="str">
+      <c r="G36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D43), "",PCR!D43)</f>
         <v/>
       </c>
-      <c r="I48" s="26" t="str">
+      <c r="H36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D51), "",PCR!D51)</f>
         <v/>
       </c>
-      <c r="J48" s="26" t="str">
+      <c r="I36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D59), "",PCR!D59)</f>
         <v/>
       </c>
-      <c r="K48" s="26" t="str">
+      <c r="J36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D67), "",PCR!D67)</f>
         <v/>
       </c>
-      <c r="L48" s="26" t="str">
+      <c r="K36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D75), "",PCR!D75)</f>
         <v/>
       </c>
-      <c r="M48" s="26" t="str">
+      <c r="L36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D83), "",PCR!D83)</f>
         <v/>
       </c>
-      <c r="N48" s="26" t="str">
+      <c r="M36" s="26" t="str">
         <f>IF(ISBLANK(PCR!D91), "",PCR!D91)</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="28" t="s">
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="26" t="str">
+      <c r="B37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D4), "",PCR!D4)</f>
         <v/>
       </c>
-      <c r="D49" s="26" t="str">
+      <c r="C37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D12), "",PCR!D12)</f>
         <v/>
       </c>
-      <c r="E49" s="26" t="str">
+      <c r="D37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D20), "",PCR!D20)</f>
         <v/>
       </c>
-      <c r="F49" s="26" t="str">
+      <c r="E37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D28), "",PCR!D28)</f>
         <v/>
       </c>
-      <c r="G49" s="26" t="str">
+      <c r="F37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D36), "",PCR!D36)</f>
         <v/>
       </c>
-      <c r="H49" s="26" t="str">
+      <c r="G37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D44), "",PCR!D44)</f>
         <v/>
       </c>
-      <c r="I49" s="26" t="str">
+      <c r="H37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D52), "",PCR!D52)</f>
         <v/>
       </c>
-      <c r="J49" s="26" t="str">
+      <c r="I37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D60), "",PCR!D60)</f>
         <v/>
       </c>
-      <c r="K49" s="26" t="str">
+      <c r="J37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D68), "",PCR!D68)</f>
         <v/>
       </c>
-      <c r="L49" s="26" t="str">
+      <c r="K37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D76), "",PCR!D76)</f>
         <v/>
       </c>
-      <c r="M49" s="26" t="str">
+      <c r="L37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D84), "",PCR!D84)</f>
         <v/>
       </c>
-      <c r="N49" s="26" t="str">
+      <c r="M37" s="26" t="str">
         <f>IF(ISBLANK(PCR!D92), "",PCR!D92)</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="28" t="s">
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="26" t="str">
+      <c r="B38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D5), "",PCR!D5)</f>
         <v/>
       </c>
-      <c r="D50" s="26" t="str">
+      <c r="C38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D13), "",PCR!D13)</f>
         <v/>
       </c>
-      <c r="E50" s="26" t="str">
+      <c r="D38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D21), "",PCR!D21)</f>
         <v/>
       </c>
-      <c r="F50" s="26" t="str">
+      <c r="E38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D29), "",PCR!D29)</f>
         <v/>
       </c>
-      <c r="G50" s="26" t="str">
+      <c r="F38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D37), "",PCR!D37)</f>
         <v/>
       </c>
-      <c r="H50" s="26" t="str">
+      <c r="G38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D45), "",PCR!D45)</f>
         <v/>
       </c>
-      <c r="I50" s="26" t="str">
+      <c r="H38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D53), "",PCR!D53)</f>
         <v/>
       </c>
-      <c r="J50" s="26" t="str">
+      <c r="I38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D61), "",PCR!D61)</f>
         <v/>
       </c>
-      <c r="K50" s="26" t="str">
+      <c r="J38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D69), "",PCR!D69)</f>
         <v/>
       </c>
-      <c r="L50" s="26" t="str">
+      <c r="K38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D77), "",PCR!D77)</f>
         <v/>
       </c>
-      <c r="M50" s="26" t="str">
+      <c r="L38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D85), "",PCR!D85)</f>
         <v/>
       </c>
-      <c r="N50" s="26" t="str">
+      <c r="M38" s="26" t="str">
         <f>IF(ISBLANK(PCR!D93), "",PCR!D93)</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="28" t="s">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="26" t="str">
+      <c r="B39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D6), "",PCR!D6)</f>
         <v/>
       </c>
-      <c r="D51" s="26" t="str">
+      <c r="C39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D14), "",PCR!D14)</f>
         <v/>
       </c>
-      <c r="E51" s="26" t="str">
+      <c r="D39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D22), "",PCR!D22)</f>
         <v/>
       </c>
-      <c r="F51" s="26" t="str">
+      <c r="E39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D30), "",PCR!D30)</f>
         <v/>
       </c>
-      <c r="G51" s="26" t="str">
+      <c r="F39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D38), "",PCR!D38)</f>
         <v/>
       </c>
-      <c r="H51" s="26" t="str">
+      <c r="G39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D46), "",PCR!D46)</f>
         <v/>
       </c>
-      <c r="I51" s="26" t="str">
+      <c r="H39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D54), "",PCR!D54)</f>
         <v/>
       </c>
-      <c r="J51" s="26" t="str">
+      <c r="I39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D62), "",PCR!D62)</f>
         <v/>
       </c>
-      <c r="K51" s="26" t="str">
+      <c r="J39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D70), "",PCR!D70)</f>
         <v/>
       </c>
-      <c r="L51" s="26" t="str">
+      <c r="K39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D78), "",PCR!D78)</f>
         <v/>
       </c>
-      <c r="M51" s="26" t="str">
+      <c r="L39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D86), "",PCR!D86)</f>
         <v/>
       </c>
-      <c r="N51" s="26" t="str">
+      <c r="M39" s="26" t="str">
         <f>IF(ISBLANK(PCR!D94), "",PCR!D94)</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="26" t="str">
+      <c r="B40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D7), "",PCR!D7)</f>
         <v/>
       </c>
-      <c r="D52" s="26" t="str">
+      <c r="C40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D15), "",PCR!D15)</f>
         <v/>
       </c>
-      <c r="E52" s="26" t="str">
+      <c r="D40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D23), "",PCR!D23)</f>
         <v/>
       </c>
-      <c r="F52" s="26" t="str">
+      <c r="E40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D31), "",PCR!D31)</f>
         <v/>
       </c>
-      <c r="G52" s="26" t="str">
+      <c r="F40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D39), "",PCR!D39)</f>
         <v/>
       </c>
-      <c r="H52" s="26" t="str">
+      <c r="G40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D47), "",PCR!D47)</f>
         <v/>
       </c>
-      <c r="I52" s="26" t="str">
+      <c r="H40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D55), "",PCR!D55)</f>
         <v/>
       </c>
-      <c r="J52" s="26" t="str">
+      <c r="I40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D63), "",PCR!D63)</f>
         <v/>
       </c>
-      <c r="K52" s="26" t="str">
+      <c r="J40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D71), "",PCR!D71)</f>
         <v/>
       </c>
-      <c r="L52" s="26" t="str">
+      <c r="K40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D79), "",PCR!D79)</f>
         <v/>
       </c>
-      <c r="M52" s="26" t="str">
+      <c r="L40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D87), "",PCR!D87)</f>
         <v/>
       </c>
-      <c r="N52" s="26" t="str">
+      <c r="M40" s="26" t="str">
         <f>IF(ISBLANK(PCR!D95), "",PCR!D95)</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="28" t="s">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="26" t="str">
+      <c r="B41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D8), "",PCR!D8)</f>
         <v/>
       </c>
-      <c r="D53" s="26" t="str">
+      <c r="C41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D16), "",PCR!D16)</f>
         <v/>
       </c>
-      <c r="E53" s="26" t="str">
+      <c r="D41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D24), "",PCR!D24)</f>
         <v/>
       </c>
-      <c r="F53" s="26" t="str">
+      <c r="E41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D32), "",PCR!D32)</f>
         <v/>
       </c>
-      <c r="G53" s="26" t="str">
+      <c r="F41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D40), "",PCR!D40)</f>
         <v/>
       </c>
-      <c r="H53" s="26" t="str">
+      <c r="G41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D48), "",PCR!D48)</f>
         <v/>
       </c>
-      <c r="I53" s="26" t="str">
+      <c r="H41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D56), "",PCR!D56)</f>
         <v/>
       </c>
-      <c r="J53" s="26" t="str">
+      <c r="I41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D64), "",PCR!D64)</f>
         <v/>
       </c>
-      <c r="K53" s="26" t="str">
+      <c r="J41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D72), "",PCR!D72)</f>
         <v/>
       </c>
-      <c r="L53" s="26" t="str">
+      <c r="K41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D80), "",PCR!D80)</f>
         <v/>
       </c>
-      <c r="M53" s="26" t="str">
+      <c r="L41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D88), "",PCR!D88)</f>
         <v/>
       </c>
-      <c r="N53" s="26" t="str">
+      <c r="M41" s="26" t="str">
         <f>IF(ISBLANK(PCR!D96), "",PCR!D96)</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="26" t="str">
+      <c r="B42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D9), "",PCR!D9)</f>
         <v/>
       </c>
-      <c r="D54" s="26" t="str">
+      <c r="C42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D17), "",PCR!D17)</f>
         <v/>
       </c>
-      <c r="E54" s="26" t="str">
+      <c r="D42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D25), "",PCR!D25)</f>
         <v/>
       </c>
-      <c r="F54" s="26" t="str">
+      <c r="E42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D33), "",PCR!D33)</f>
         <v/>
       </c>
-      <c r="G54" s="26" t="str">
+      <c r="F42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D41), "",PCR!D41)</f>
         <v/>
       </c>
-      <c r="H54" s="26" t="str">
+      <c r="G42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D49), "",PCR!D49)</f>
         <v/>
       </c>
-      <c r="I54" s="26" t="str">
+      <c r="H42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D57), "",PCR!D57)</f>
         <v/>
       </c>
-      <c r="J54" s="26" t="str">
+      <c r="I42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D65), "",PCR!D65)</f>
         <v/>
       </c>
-      <c r="K54" s="26" t="str">
+      <c r="J42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D73), "",PCR!D73)</f>
         <v/>
       </c>
-      <c r="L54" s="26" t="str">
+      <c r="K42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D81), "",PCR!D81)</f>
         <v/>
       </c>
-      <c r="M54" s="26" t="str">
+      <c r="L42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D89), "",PCR!D89)</f>
         <v/>
       </c>
-      <c r="N54" s="26" t="str">
+      <c r="M42" s="26" t="str">
         <f>IF(ISBLANK(PCR!D97), "",PCR!D97)</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="28" t="s">
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="26" t="str">
+      <c r="B43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D10), "",PCR!D10)</f>
         <v/>
       </c>
-      <c r="D55" s="26" t="str">
+      <c r="C43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D18), "",PCR!D18)</f>
         <v/>
       </c>
-      <c r="E55" s="26" t="str">
+      <c r="D43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D26), "",PCR!D26)</f>
         <v/>
       </c>
-      <c r="F55" s="26" t="str">
+      <c r="E43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D34), "",PCR!D34)</f>
         <v/>
       </c>
-      <c r="G55" s="26" t="str">
+      <c r="F43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D42), "",PCR!D42)</f>
         <v/>
       </c>
-      <c r="H55" s="26" t="str">
+      <c r="G43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D50), "",PCR!D50)</f>
         <v/>
       </c>
-      <c r="I55" s="26" t="str">
+      <c r="H43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D58), "",PCR!D58)</f>
         <v/>
       </c>
-      <c r="J55" s="26" t="str">
+      <c r="I43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D66), "",PCR!D66)</f>
         <v/>
       </c>
-      <c r="K55" s="26" t="str">
+      <c r="J43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D74), "",PCR!D74)</f>
         <v/>
       </c>
-      <c r="L55" s="26" t="str">
+      <c r="K43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D82), "",PCR!D82)</f>
         <v/>
       </c>
-      <c r="M55" s="26" t="str">
+      <c r="L43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D90), "",PCR!D90)</f>
         <v/>
       </c>
-      <c r="N55" s="26" t="str">
+      <c r="M43" s="26" t="str">
         <f>IF(ISBLANK(PCR!D98), "",PCR!D98)</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="8"/>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="117">
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:L18"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="L5:M6"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="N37:N39"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E21:F21"/>
+  <mergeCells count="69">
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C17:K18"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2:D4 D11 D14:D17">
-    <cfRule type="expression" dxfId="29" priority="11">
-      <formula>COUNTIF(D2,"")</formula>
+  <conditionalFormatting sqref="A25:C27">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>A25="-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D8">
-    <cfRule type="expression" dxfId="28" priority="1">
-      <formula>COUNTIF(D7,"")</formula>
+  <conditionalFormatting sqref="C2:C4 C11 C14:C17">
+    <cfRule type="expression" dxfId="8" priority="17">
+      <formula>COUNTIF(C2,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." sqref="D10 D9:G9" xr:uid="{B2B8BFB3-0AE7-4ECF-A2D1-0DE481577069}"/>
+  <conditionalFormatting sqref="C7:C8">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>COUNTIF(C7,"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:E22">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
+      <formula>LEN(TRIM(D22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:E27">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>A25="-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:G27">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>$A22="-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:M26">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+      <formula>J22=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M22:M26">
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>LEN(M22)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." sqref="C10 C9:F9" xr:uid="{B2B8BFB3-0AE7-4ECF-A2D1-0DE481577069}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:F4" xr:uid="{9E3F1EDD-ECC0-4744-B8A4-53A5A89BEC01}">
+      <formula1>LEN(C4)=3</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Format" error="Exp Numbers should be three digits long" sqref="C5:F5" xr:uid="{3305B6EA-24D3-4F5D-A2AC-BB3F2ACD221C}"/>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -4397,25 +4061,25 @@
           <x14:formula1>
             <xm:f>reference!$E$3:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:G11</xm:sqref>
+          <xm:sqref>C11:F11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E7C7338-D4B5-4229-8F49-1913883BAA1F}">
           <x14:formula1>
             <xm:f>reference!$I$3:$I$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D3</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACDC75C9-791B-4E82-A9A3-D2BDFD36107F}">
           <x14:formula1>
             <xm:f>reference!$L$3:$L$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D7:G7</xm:sqref>
+          <xm:sqref>C7:F7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7DC0BE7F-A938-49D1-8508-05D8BFD25456}">
           <x14:formula1>
             <xm:f>reference!$E$14:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:G15</xm:sqref>
+          <xm:sqref>C15:F15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4447,21 +4111,21 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="54"/>
       <c r="B1" s="54"/>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
       <c r="F1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="111"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="109"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
@@ -4477,7 +4141,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F2" s="51" t="s">
         <v>186</v>
@@ -6827,12 +6491,12 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C3:E98">
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I98 K3:K98 C3:F98">
-    <cfRule type="expression" dxfId="26" priority="10">
+  <conditionalFormatting sqref="C3:F98 H3:I98 K3:K98">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>COUNTIF(C3,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6901,10 +6565,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7012,7 +6676,7 @@
         <v>214</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I5" s="53" t="s">
         <v>253</v>
@@ -7032,13 +6696,13 @@
         <v>23</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I6" s="53"/>
       <c r="J6" s="53"/>
@@ -7049,16 +6713,16 @@
         <v>172</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I7" s="53"/>
       <c r="J7" s="53"/>
@@ -7085,7 +6749,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E10" t="s">
         <v>257</v>
@@ -7126,7 +6790,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -7134,24 +6798,531 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="5:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="70" t="str">
+        <f t="shared" ref="E24:E29" si="0">IF(pcr_enzyme=$E$14,E32,IF(pcr_enzyme=$E$15,E40,IF(pcr_enzyme=$E$16,E48,"")))</f>
+        <v/>
+      </c>
+      <c r="F24" s="70" t="str">
+        <f>IF(template_vol="","",template_vol)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F25" s="70" t="str">
+        <f>IF(pcr_enzyme=$E$14,F33,IF(pcr_enzyme=$E$15,F41,IF(pcr_enzyme=$E$16,F49,"")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F26" s="70" t="str">
+        <f>IF(pcr_enzyme=$E$14,F34,IF(pcr_enzyme=$E$15,F42,IF(pcr_enzyme=$E$16,F50,"")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F27" s="70" t="str">
+        <f>IF(pcr_enzyme=$E$14,F35,IF(pcr_enzyme=$E$15,F43,IF(pcr_enzyme=$E$16,F51,"")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F28" s="70" t="str">
+        <f>IF(pcr_enzyme=$E$14,F36,IF(pcr_enzyme=$E$15,F44,IF(pcr_enzyme=$E$16,F52,"")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F29" s="70" t="str">
+        <f>IF(E29="","",SUM(25-SUM(F24:F28)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32">
+        <f>template_vol</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>259</v>
+      </c>
+      <c r="F33">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>254</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40">
+        <f>template_vol</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>283</v>
+      </c>
+      <c r="F41">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <f>SUM(25-SUM(F40:F42))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="23"/>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>217</v>
+      </c>
+      <c r="F48">
+        <f>template_vol</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>218</v>
+      </c>
+      <c r="F49">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!E63,IF(exp_assay=$E$5,E70,IF(exp_assay=$E$6,E76,IF(exp_assay=$E$7,E83,""))))</f>
+        <v/>
+      </c>
+      <c r="F56" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!F63,IF(exp_assay=$E$5,F70,IF(exp_assay=$E$6,F76,IF(exp_assay=$E$7,F83,""))))</f>
+        <v/>
+      </c>
+      <c r="G56" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!G63,IF(exp_assay=$E$5,G70,IF(exp_assay=$E$6,G76,IF(exp_assay=$E$7,G83,""))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!E64,IF(exp_assay=$E$5,E71,IF(exp_assay=$E$6,E77,IF(exp_assay=$E$7,E84,""))))</f>
+        <v/>
+      </c>
+      <c r="F57" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!F64,IF(exp_assay=$E$5,F71,IF(exp_assay=$E$6,F77,IF(exp_assay=$E$7,F84,""))))</f>
+        <v/>
+      </c>
+      <c r="G57" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!G64,IF(exp_assay=$E$5,G71,IF(exp_assay=$E$6,G77,IF(exp_assay=$E$7,G84,""))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!E65,IF(exp_assay=$E$5,E72,IF(exp_assay=$E$6,E78,IF(exp_assay=$E$7,E85,""))))</f>
+        <v/>
+      </c>
+      <c r="F58" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!F65,IF(exp_assay=$E$5,F72,IF(exp_assay=$E$6,F78,IF(exp_assay=$E$7,F85,""))))</f>
+        <v/>
+      </c>
+      <c r="G58" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!G65,IF(exp_assay=$E$5,G72,IF(exp_assay=$E$6,G78,IF(exp_assay=$E$7,G85,""))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E59" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!E66,IF(exp_assay=$E$5,E73,IF(exp_assay=$E$6,E79,IF(exp_assay=$E$7,E86,""))))</f>
+        <v/>
+      </c>
+      <c r="F59" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!F66,IF(exp_assay=$E$5,F73,IF(exp_assay=$E$6,F79,IF(exp_assay=$E$7,F86,""))))</f>
+        <v/>
+      </c>
+      <c r="G59" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!G66,IF(exp_assay=$E$5,G73,IF(exp_assay=$E$6,G79,IF(exp_assay=$E$7,G86,""))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E60" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!E67,IF(exp_assay=$E$5,E74,IF(exp_assay=$E$6,E80,IF(exp_assay=$E$7,E87,""))))</f>
+        <v/>
+      </c>
+      <c r="F60" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!F67,IF(exp_assay=$E$5,F74,IF(exp_assay=$E$6,F80,IF(exp_assay=$E$7,F87,""))))</f>
+        <v/>
+      </c>
+      <c r="G60" s="70" t="str">
+        <f>IF(OR(exp_assay=$E$3,exp_assay=$E$4),reference!G67,IF(exp_assay=$E$5,G74,IF(exp_assay=$E$6,G80,IF(exp_assay=$E$7,G87,""))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>93</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>98</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>50</v>
+      </c>
+      <c r="F65" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>60</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>60</v>
+      </c>
+      <c r="F67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="23" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>95</v>
+      </c>
+      <c r="F70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>95</v>
+      </c>
+      <c r="F71" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>278</v>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>98</v>
+      </c>
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>60</v>
+      </c>
+      <c r="F73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E75" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>93</v>
+      </c>
+      <c r="F76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>98</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>50</v>
+      </c>
+      <c r="F78" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>60</v>
+      </c>
+      <c r="F79" t="s">
+        <v>18</v>
+      </c>
+      <c r="G79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>60</v>
+      </c>
+      <c r="F80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E82" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>93</v>
+      </c>
+      <c r="F83" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>98</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>50</v>
+      </c>
+      <c r="F85" t="s">
+        <v>17</v>
+      </c>
+      <c r="G85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>60</v>
+      </c>
+      <c r="F86" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>60</v>
+      </c>
+      <c r="F87" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -7171,7 +7342,9 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7390,10 +7563,10 @@
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7402,11 +7575,11 @@
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="7" width="12.125" customWidth="1"/>
     <col min="8" max="8" width="31.625" customWidth="1"/>
-    <col min="9" max="12" width="12.125" customWidth="1"/>
-    <col min="13" max="13" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="12.125" customWidth="1"/>
+    <col min="14" max="14" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -7444,10 +7617,13 @@
         <v>177</v>
       </c>
       <c r="M1" t="s">
+        <v>281</v>
+      </c>
+      <c r="N1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(LEN(exp_id)=0,"",exp_id)</f>
         <v/>
@@ -7466,7 +7642,7 @@
       </c>
       <c r="E2">
         <f>IF(LEN(exp_version)=0,"",exp_version)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="str">
         <f>IF(LEN(exp_assay)=0,"",exp_assay)</f>
@@ -7497,12 +7673,16 @@
         <v/>
       </c>
       <c r="M2" t="str">
+        <f>IF(LEN(template_vol)=0,"",template_vol)</f>
+        <v/>
+      </c>
+      <c r="N2" t="str">
         <f>IF(pcr_enzyme=0,"",pcr_enzyme)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="38/yEmFxISJT1sY8Z2orWimA3cEyEJZ0P1DXv9yg/yio8fwMqxXUFmuz44H2ybJU+WY3aTg/nsN+nWFHZW5RJw==" saltValue="dQEaq+u+fjoGcyZDox/wsw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vph7DaMh3SyowaNNd8/hWiOan38yUHTDW1w5tTlbGEdRpJuRTmeOvrHT9rmEAjHGl0Numj/KRrc+UvQhk/Kdtg==" saltValue="/M7Z5DLigzvvgEv+lbbvig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7538,7 +7718,7 @@
         <v>182</v>
       </c>
       <c r="C1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D1" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Corrected to 0.5x post-pcr clean-up
</commit_message>
<xml_diff>
--- a/templates/NOMADS_PCR_Worksheet.xlsx
+++ b/templates/NOMADS_PCR_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D19743-246C-4057-B056-580D6BED0E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B96FEF-95F2-4CF4-A747-AB3CC742A90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" activeTab="4" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -159,30 +159,6 @@
     <t>Overage</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">2. Clean-up with 23 µl AMPPure beads (1X ratio), mix and incubate at RT for 5 min. Pellet on magnet for 8 min and wash 2 x 200 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>l 80%  fresh EtoH, spin, dry, then re-suspend in 15 µl EB and transfer to fresh tube / well</t>
-    </r>
-  </si>
-  <si>
     <t>Look-ups</t>
   </si>
   <si>
@@ -612,9 +588,6 @@
   </si>
   <si>
     <t>NOMADS PCR Worksheet</t>
-  </si>
-  <si>
-    <t>1. Run 2 µl of PCR product on a 1% agarose gel, picture and annotate it</t>
   </si>
   <si>
     <t>(Enter in Gel Image Tab)</t>
@@ -1234,6 +1207,12 @@
   <si>
     <t>Rxn volume</t>
   </si>
+  <si>
+    <t>1. Run 1 µl of PCR product on a 1% agarose gel, picture and annotate it</t>
+  </si>
+  <si>
+    <t>2. Clean-up with 12 µl (0.5X) AMPPure beads per sample, mix and incubate at RT for 5 min. Pellet on magnet for 8 min and wash 2 x 200 µl 80%  fresh EtoH, spin, dry, then re-suspend in 15 µl EB and transfer to fresh tube / well</t>
+  </si>
 </sst>
 </file>
 
@@ -1244,7 +1223,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1300,12 +1279,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1834,7 +1807,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1854,14 +1827,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1888,27 +1861,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1955,7 +1928,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1963,19 +1936,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2051,7 +2024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2112,7 +2085,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2139,7 +2112,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3149,8 +3122,8 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3160,7 +3133,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="102"/>
@@ -3177,7 +3150,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="93"/>
       <c r="C2" s="105"/>
@@ -3185,17 +3158,17 @@
       <c r="E2" s="105"/>
       <c r="F2" s="105"/>
       <c r="G2" s="103" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="103"/>
       <c r="K2" s="110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="93"/>
       <c r="C3" s="106"/>
@@ -3203,7 +3176,7 @@
       <c r="E3" s="106"/>
       <c r="F3" s="106"/>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K3" s="111" t="s">
         <v>3</v>
@@ -3212,7 +3185,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="93"/>
       <c r="C4" s="109"/>
@@ -3220,7 +3193,7 @@
       <c r="E4" s="109"/>
       <c r="F4" s="109"/>
       <c r="G4" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K4" s="112" t="s">
         <v>4</v>
@@ -3229,7 +3202,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="95" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="104"/>
       <c r="C5" s="107" t="str">
@@ -3240,16 +3213,16 @@
       <c r="E5" s="107"/>
       <c r="F5" s="107"/>
       <c r="G5" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K5" s="113" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L5" s="113"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="104"/>
       <c r="C6" s="108" t="str">
@@ -3265,7 +3238,7 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="115" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B7" s="115"/>
       <c r="C7" s="97"/>
@@ -3273,12 +3246,12 @@
       <c r="E7" s="97"/>
       <c r="F7" s="97"/>
       <c r="G7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="115" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8" s="115"/>
       <c r="C8" s="97"/>
@@ -3286,12 +3259,12 @@
       <c r="E8" s="97"/>
       <c r="F8" s="97"/>
       <c r="G8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="116" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9" s="116"/>
       <c r="C9" s="118" t="str">
@@ -3302,12 +3275,12 @@
       <c r="E9" s="118"/>
       <c r="F9" s="118"/>
       <c r="G9" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="116" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10" s="116"/>
       <c r="C10" s="117" t="str">
@@ -3322,7 +3295,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="93"/>
       <c r="C11" s="119"/>
@@ -3330,12 +3303,12 @@
       <c r="E11" s="119"/>
       <c r="F11" s="119"/>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B12" s="95"/>
       <c r="C12" s="96" t="str">
@@ -3346,12 +3319,12 @@
       <c r="E12" s="96"/>
       <c r="F12" s="96"/>
       <c r="G12" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="95" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" s="95"/>
       <c r="C13" s="96" t="str">
@@ -3362,12 +3335,12 @@
       <c r="E13" s="96"/>
       <c r="F13" s="96"/>
       <c r="G13" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="93"/>
       <c r="C14" s="97"/>
@@ -3375,12 +3348,12 @@
       <c r="E14" s="97"/>
       <c r="F14" s="97"/>
       <c r="G14" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="92" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B15" s="93"/>
       <c r="C15" s="97"/>
@@ -3388,12 +3361,12 @@
       <c r="E15" s="97"/>
       <c r="F15" s="97"/>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="93"/>
       <c r="C16" s="97"/>
@@ -3404,7 +3377,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="92" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B17" s="93"/>
       <c r="C17" s="100"/>
@@ -3442,7 +3415,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="12" t="s">
@@ -3483,7 +3456,7 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="86" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B22" s="86"/>
       <c r="C22" s="86"/>
@@ -3708,7 +3681,7 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -3718,14 +3691,14 @@
       <c r="G30"/>
       <c r="H30"/>
       <c r="K30" s="85" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L30" s="85"/>
       <c r="M30" s="85"/>
     </row>
     <row r="31" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="103" t="s">
-        <v>25</v>
+        <v>291</v>
       </c>
       <c r="B31" s="103"/>
       <c r="C31" s="103"/>
@@ -3742,7 +3715,7 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3752,7 +3725,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="8"/>
       <c r="K32" s="94" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L32" s="94"/>
       <c r="M32" s="94"/>
@@ -3772,7 +3745,7 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -3822,7 +3795,7 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="21" t="str">
         <f>PCR!$G3</f>
@@ -3875,7 +3848,7 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="21" t="str">
         <f>PCR!$G4</f>
@@ -3928,7 +3901,7 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="21" t="str">
         <f>PCR!$G5</f>
@@ -3981,7 +3954,7 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="21" t="str">
         <f>PCR!$G6</f>
@@ -4034,7 +4007,7 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="21" t="str">
         <f>PCR!$G7</f>
@@ -4087,7 +4060,7 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="21" t="str">
         <f>PCR!$G8</f>
@@ -4140,7 +4113,7 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21" t="str">
         <f>PCR!$G9</f>
@@ -4193,7 +4166,7 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="21" t="str">
         <f>PCR!$G10</f>
@@ -4249,7 +4222,6 @@
       <c r="B44" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="72">
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="A31:M31"/>
@@ -4484,13 +4456,13 @@
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>5</v>
@@ -4499,28 +4471,28 @@
         <v>21</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I2" s="60" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J2" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="60" t="s">
-        <v>158</v>
-      </c>
       <c r="M2" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4532,7 +4504,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="63"/>
@@ -4563,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
@@ -4594,7 +4566,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
@@ -4625,7 +4597,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -4656,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
@@ -4687,7 +4659,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
@@ -4718,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -4749,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
@@ -4780,7 +4752,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
@@ -4811,7 +4783,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
@@ -4842,7 +4814,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -4873,7 +4845,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
@@ -4904,7 +4876,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
@@ -4935,7 +4907,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -4966,7 +4938,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -4997,7 +4969,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="73"/>
       <c r="E18" s="73"/>
@@ -5028,7 +5000,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
@@ -5059,7 +5031,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5090,7 +5062,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -5121,7 +5093,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -5152,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -5183,7 +5155,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -5214,7 +5186,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
@@ -5245,7 +5217,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="73"/>
       <c r="E26" s="73"/>
@@ -5276,7 +5248,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
@@ -5307,7 +5279,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -5338,7 +5310,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -5369,7 +5341,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -5400,7 +5372,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -5431,7 +5403,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
@@ -5462,7 +5434,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
@@ -5493,7 +5465,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="73"/>
       <c r="E34" s="73"/>
@@ -5524,7 +5496,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
@@ -5555,7 +5527,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -5586,7 +5558,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -5617,7 +5589,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -5648,7 +5620,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -5679,7 +5651,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
@@ -5710,7 +5682,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
@@ -5741,7 +5713,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="73"/>
       <c r="E42" s="73"/>
@@ -5772,7 +5744,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="63"/>
       <c r="E43" s="63"/>
@@ -5803,7 +5775,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
@@ -5834,7 +5806,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
@@ -5865,7 +5837,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
@@ -5896,7 +5868,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
@@ -5927,7 +5899,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
@@ -5958,7 +5930,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
@@ -5989,7 +5961,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" s="73"/>
       <c r="E50" s="73"/>
@@ -6020,7 +5992,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
@@ -6051,7 +6023,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
@@ -6082,7 +6054,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
@@ -6113,7 +6085,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
@@ -6144,7 +6116,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
@@ -6175,7 +6147,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
@@ -6206,7 +6178,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="24"/>
       <c r="E57" s="24"/>
@@ -6237,7 +6209,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" s="73"/>
       <c r="E58" s="73"/>
@@ -6268,7 +6240,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59" s="63"/>
       <c r="E59" s="63"/>
@@ -6299,7 +6271,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="24"/>
@@ -6330,7 +6302,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D61" s="24"/>
       <c r="E61" s="24"/>
@@ -6361,7 +6333,7 @@
         <v>8</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D62" s="24"/>
       <c r="E62" s="24"/>
@@ -6392,7 +6364,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D63" s="24"/>
       <c r="E63" s="24"/>
@@ -6423,7 +6395,7 @@
         <v>8</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D64" s="24"/>
       <c r="E64" s="24"/>
@@ -6454,7 +6426,7 @@
         <v>8</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D65" s="24"/>
       <c r="E65" s="24"/>
@@ -6485,7 +6457,7 @@
         <v>8</v>
       </c>
       <c r="C66" s="81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D66" s="73"/>
       <c r="E66" s="73"/>
@@ -6516,7 +6488,7 @@
         <v>9</v>
       </c>
       <c r="C67" s="62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D67" s="63"/>
       <c r="E67" s="63"/>
@@ -6547,7 +6519,7 @@
         <v>9</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D68" s="24"/>
       <c r="E68" s="24"/>
@@ -6578,7 +6550,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D69" s="24"/>
       <c r="E69" s="24"/>
@@ -6609,7 +6581,7 @@
         <v>9</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D70" s="24"/>
       <c r="E70" s="24"/>
@@ -6640,7 +6612,7 @@
         <v>9</v>
       </c>
       <c r="C71" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
@@ -6671,7 +6643,7 @@
         <v>9</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D72" s="24"/>
       <c r="E72" s="24"/>
@@ -6702,7 +6674,7 @@
         <v>9</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D73" s="24"/>
       <c r="E73" s="24"/>
@@ -6733,7 +6705,7 @@
         <v>9</v>
       </c>
       <c r="C74" s="81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D74" s="73"/>
       <c r="E74" s="73"/>
@@ -6764,7 +6736,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D75" s="63"/>
       <c r="E75" s="63"/>
@@ -6795,7 +6767,7 @@
         <v>10</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D76" s="24"/>
       <c r="E76" s="24"/>
@@ -6826,7 +6798,7 @@
         <v>10</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D77" s="24"/>
       <c r="E77" s="24"/>
@@ -6857,7 +6829,7 @@
         <v>10</v>
       </c>
       <c r="C78" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D78" s="24"/>
       <c r="E78" s="24"/>
@@ -6888,7 +6860,7 @@
         <v>10</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D79" s="24"/>
       <c r="E79" s="24"/>
@@ -6919,7 +6891,7 @@
         <v>10</v>
       </c>
       <c r="C80" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D80" s="24"/>
       <c r="E80" s="24"/>
@@ -6950,7 +6922,7 @@
         <v>10</v>
       </c>
       <c r="C81" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D81" s="24"/>
       <c r="E81" s="24"/>
@@ -6981,7 +6953,7 @@
         <v>10</v>
       </c>
       <c r="C82" s="81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D82" s="73"/>
       <c r="E82" s="73"/>
@@ -7012,7 +6984,7 @@
         <v>11</v>
       </c>
       <c r="C83" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D83" s="63"/>
       <c r="E83" s="63"/>
@@ -7043,7 +7015,7 @@
         <v>11</v>
       </c>
       <c r="C84" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D84" s="24"/>
       <c r="E84" s="24"/>
@@ -7074,7 +7046,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D85" s="24"/>
       <c r="E85" s="24"/>
@@ -7105,7 +7077,7 @@
         <v>11</v>
       </c>
       <c r="C86" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D86" s="24"/>
       <c r="E86" s="24"/>
@@ -7136,7 +7108,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D87" s="24"/>
       <c r="E87" s="24"/>
@@ -7167,7 +7139,7 @@
         <v>11</v>
       </c>
       <c r="C88" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D88" s="24"/>
       <c r="E88" s="24"/>
@@ -7198,7 +7170,7 @@
         <v>11</v>
       </c>
       <c r="C89" s="45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D89" s="24"/>
       <c r="E89" s="24"/>
@@ -7229,7 +7201,7 @@
         <v>11</v>
       </c>
       <c r="C90" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D90" s="73"/>
       <c r="E90" s="73"/>
@@ -7260,7 +7232,7 @@
         <v>12</v>
       </c>
       <c r="C91" s="62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D91" s="63"/>
       <c r="E91" s="63"/>
@@ -7291,7 +7263,7 @@
         <v>12</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D92" s="24"/>
       <c r="E92" s="24"/>
@@ -7322,7 +7294,7 @@
         <v>12</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D93" s="24"/>
       <c r="E93" s="24"/>
@@ -7353,7 +7325,7 @@
         <v>12</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D94" s="24"/>
       <c r="E94" s="24"/>
@@ -7384,7 +7356,7 @@
         <v>12</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D95" s="24"/>
       <c r="E95" s="24"/>
@@ -7415,7 +7387,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D96" s="24"/>
       <c r="E96" s="24"/>
@@ -7446,7 +7418,7 @@
         <v>12</v>
       </c>
       <c r="C97" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D97" s="24"/>
       <c r="E97" s="24"/>
@@ -7477,7 +7449,7 @@
         <v>12</v>
       </c>
       <c r="C98" s="81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D98" s="73"/>
       <c r="E98" s="73"/>
@@ -7689,10 +7661,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -7710,7 +7682,7 @@
   </sheetPr>
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -7731,11 +7703,11 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="4"/>
       <c r="I1" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7745,107 +7717,107 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="E2" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>143</v>
-      </c>
       <c r="I2" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>153</v>
-      </c>
       <c r="L2" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C3" s="6"/>
       <c r="E3" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="G3" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>146</v>
-      </c>
       <c r="I3" s="42" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D4" s="6"/>
       <c r="E4" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="G4" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>149</v>
-      </c>
       <c r="I4" s="42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="6"/>
       <c r="E5" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I6" s="42"/>
       <c r="J6" s="42"/>
@@ -7853,19 +7825,19 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>9</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I7" s="42"/>
       <c r="J7" s="42"/>
@@ -7881,95 +7853,95 @@
     </row>
     <row r="9" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I12" s="27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="53" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F24" s="53" t="str">
         <f>IF(pcr_enzyme=$E$14,F32,IF(pcr_enzyme=$E$15,F42,IF(pcr_enzyme=$E$16,F52,"")))</f>
@@ -8028,13 +8000,13 @@
     </row>
     <row r="31" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E31" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F32">
         <v>8</v>
@@ -8042,7 +8014,7 @@
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F33">
         <f>SUM(F35:F38)</f>
@@ -8051,7 +8023,7 @@
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F34">
         <v>25</v>
@@ -8059,7 +8031,7 @@
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F35">
         <v>0.3</v>
@@ -8067,7 +8039,7 @@
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F36">
         <v>0.75</v>
@@ -8075,7 +8047,7 @@
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F37">
         <v>5</v>
@@ -8101,13 +8073,13 @@
     </row>
     <row r="41" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E41" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F42">
         <v>8</v>
@@ -8115,7 +8087,7 @@
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F43">
         <f>SUM(F45:F46)</f>
@@ -8124,7 +8096,7 @@
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F44">
         <v>25</v>
@@ -8132,7 +8104,7 @@
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F45">
         <v>15.5</v>
@@ -8167,13 +8139,13 @@
     </row>
     <row r="51" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E51" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F51" s="18"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F52">
         <v>5</v>
@@ -8181,7 +8153,7 @@
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F53">
         <f>SUM(F55:F56)</f>
@@ -8190,7 +8162,7 @@
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -8198,7 +8170,7 @@
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F55">
         <v>14.5</v>
@@ -8233,7 +8205,7 @@
     </row>
     <row r="61" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E61" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
@@ -8338,7 +8310,7 @@
     </row>
     <row r="70" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E70" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
@@ -8348,7 +8320,7 @@
         <v>93</v>
       </c>
       <c r="F71" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G71" s="54"/>
     </row>
@@ -8406,12 +8378,12 @@
         <v>8</v>
       </c>
       <c r="F77" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="78" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E78" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
@@ -8421,7 +8393,7 @@
         <v>95</v>
       </c>
       <c r="F79" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
@@ -8440,7 +8412,7 @@
         <v>16</v>
       </c>
       <c r="G81" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
@@ -8451,7 +8423,7 @@
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
@@ -8467,7 +8439,7 @@
         <v>8</v>
       </c>
       <c r="F84" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
@@ -8475,7 +8447,7 @@
     </row>
     <row r="86" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E86" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F86" s="18"/>
       <c r="G86" s="18"/>
@@ -8485,7 +8457,7 @@
         <v>93</v>
       </c>
       <c r="F87" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G87" s="54"/>
     </row>
@@ -8543,12 +8515,12 @@
         <v>8</v>
       </c>
       <c r="F93" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="94" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E94" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F94" s="18"/>
       <c r="G94" s="18"/>
@@ -8558,7 +8530,7 @@
         <v>93</v>
       </c>
       <c r="F95" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G95" s="54"/>
     </row>
@@ -8616,12 +8588,12 @@
         <v>8</v>
       </c>
       <c r="F101" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E103" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.25">
@@ -8651,7 +8623,7 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -8668,14 +8640,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -8687,24 +8659,24 @@
     </row>
     <row r="4" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A4" s="33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A5" s="31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A6" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C6" s="31"/>
     </row>
@@ -8713,49 +8685,49 @@
         <v>23</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C7" s="31"/>
     </row>
     <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A9" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C9" s="31"/>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A11" s="36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="31"/>
@@ -8767,70 +8739,70 @@
     </row>
     <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="31" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
     </row>
     <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A19" s="32" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A21" s="32" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
     </row>
     <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A23" s="38" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
@@ -8842,21 +8814,21 @@
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A25" s="33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A26" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -8890,46 +8862,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
         <v>168</v>
       </c>
-      <c r="B1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1" t="s">
-        <v>170</v>
-      </c>
       <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" t="s">
         <v>175</v>
       </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K1" t="s">
-        <v>194</v>
-      </c>
-      <c r="L1" t="s">
-        <v>177</v>
-      </c>
       <c r="M1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -9021,25 +8993,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to better merge data within classes
</commit_message>
<xml_diff>
--- a/templates/NOMADS_PCR_Worksheet.xlsx
+++ b/templates/NOMADS_PCR_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68EFD04-E32C-47AE-8262-7532CC8C1C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E000A9-6C4B-4103-8D1C-D3212E051F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29100" activeTab="4" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29670" windowHeight="19260" activeTab="4" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="6" r:id="rId1"/>
@@ -1175,9 +1175,6 @@
     <t>Selected Primer Set</t>
   </si>
   <si>
-    <t>template_vol</t>
-  </si>
-  <si>
     <t>Selected polymerase</t>
   </si>
   <si>
@@ -1218,6 +1215,9 @@
   </si>
   <si>
     <t>Post-PCR clean-up target [DNA]</t>
+  </si>
+  <si>
+    <t>pcr_template_vol</t>
   </si>
 </sst>
 </file>
@@ -2042,44 +2042,30 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2087,8 +2073,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2123,38 +2138,23 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2806,7 +2806,7 @@
     <tableColumn id="9" xr3:uid="{5C17D014-189E-43E2-A899-4574390B7A58}" name="pcr_targetpanel">
       <calculatedColumnFormula>IF(LEN(pcr_targetpanel)=0,"",pcr_targetpanel)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{B1248788-8BBB-4F40-90D1-7B509917F807}" name="template_vol">
+    <tableColumn id="14" xr3:uid="{B1248788-8BBB-4F40-90D1-7B509917F807}" name="pcr_template_vol">
       <calculatedColumnFormula>IF(LEN(template_vol)=0,"",template_vol)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{4786D324-56A9-420B-A7CB-8083E29E50BD}" name="pcr_enzyme">
@@ -3160,276 +3160,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="103" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="93" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="86" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="104" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="K2" s="106" t="s">
+      <c r="H2" s="104"/>
+      <c r="K2" s="111" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="106"/>
+      <c r="L2" s="111"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="93" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
       <c r="G3" t="s">
         <v>155</v>
       </c>
-      <c r="K3" s="107" t="s">
+      <c r="K3" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="107"/>
+      <c r="L3" s="112"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="93" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
       <c r="G4" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="K4" s="108" t="s">
+      <c r="K4" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="108"/>
+      <c r="L4" s="113"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="103" t="str">
+      <c r="B5" s="105"/>
+      <c r="C5" s="108" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("PC",VLOOKUP(C3,reference!I3:J8,2,FALSE),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="K5" s="109" t="s">
+      <c r="K5" s="114" t="s">
         <v>197</v>
       </c>
-      <c r="L5" s="109"/>
+      <c r="L5" s="114"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="104" t="str">
+      <c r="B6" s="105"/>
+      <c r="C6" s="109" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),LEN(C5)=0),"",CONCATENATE(C2,"_PCR_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
       <c r="G6" s="17"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
       <c r="G7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="116" t="s">
         <v>199</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
       <c r="G8" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="117" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="91" t="str">
+      <c r="B9" s="117"/>
+      <c r="C9" s="119" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
       <c r="G9" s="15" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="117" t="s">
         <v>203</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="90" t="str">
+      <c r="B10" s="117"/>
+      <c r="C10" s="118" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary,".xlsx"))</f>
         <v/>
       </c>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="93" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
       <c r="G11" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="93" t="str">
+      <c r="B12" s="96"/>
+      <c r="C12" s="97" t="str">
         <f>IF(ISBLANK(C11),"",VLOOKUP(C11,tbl_Assays[],2,FALSE))</f>
         <v/>
       </c>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="97"/>
       <c r="G12" s="15" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="96" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="93" t="str">
+      <c r="B13" s="96"/>
+      <c r="C13" s="97" t="str">
         <f>IF(ISBLANK(C11),"",VLOOKUP(C11,tbl_Assays[],3,FALSE))</f>
         <v/>
       </c>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
       <c r="G13" s="15" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="98"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
       <c r="G14" s="15" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
       <c r="G15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="98"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
       <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="93" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="101"/>
+      <c r="J17" s="101"/>
+      <c r="K17" s="101"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="101"/>
+      <c r="J18" s="101"/>
+      <c r="K18" s="101"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -3456,25 +3456,25 @@
       <c r="H20"/>
     </row>
     <row r="21" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="111" t="s">
+      <c r="A21" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="110" t="s">
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110" t="str">
+      <c r="E21" s="99"/>
+      <c r="F21" s="99" t="str">
         <f>CONCATENATE("MM x",exp_rxns, " (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G21" s="110"/>
+      <c r="G21" s="99"/>
       <c r="H21" s="8"/>
-      <c r="J21" s="113" t="s">
+      <c r="J21" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="113"/>
+      <c r="K21" s="102"/>
       <c r="L21" s="48" t="s">
         <v>14</v>
       </c>
@@ -3483,24 +3483,24 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="87" t="s">
         <v>215</v>
       </c>
-      <c r="B22" s="95"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="119" t="s">
+      <c r="B22" s="87"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="119"/>
+      <c r="G22" s="89"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
-      <c r="J22" s="116" t="str">
+      <c r="J22" s="92" t="str">
         <f>reference!E62</f>
         <v/>
       </c>
-      <c r="K22" s="116"/>
+      <c r="K22" s="92"/>
       <c r="L22" s="50" t="str">
         <f>reference!F62</f>
         <v/>
@@ -3511,29 +3511,29 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="str">
+      <c r="A23" s="87" t="str">
         <f>reference!E25</f>
         <v/>
       </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="94" t="str">
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="91" t="str">
         <f>reference!F25</f>
         <v/>
       </c>
-      <c r="E23" s="94"/>
-      <c r="F23" s="115" t="str">
+      <c r="E23" s="91"/>
+      <c r="F23" s="88" t="str">
         <f>IFERROR(SUM(D23*exp_rxns*(1+$D$20)),"")</f>
         <v/>
       </c>
-      <c r="G23" s="115"/>
+      <c r="G23" s="88"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
-      <c r="J23" s="116" t="str">
+      <c r="J23" s="92" t="str">
         <f>reference!E63</f>
         <v/>
       </c>
-      <c r="K23" s="116"/>
+      <c r="K23" s="92"/>
       <c r="L23" s="50" t="str">
         <f>reference!F63</f>
         <v/>
@@ -3544,29 +3544,29 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="str">
+      <c r="A24" s="87" t="str">
         <f>reference!E26</f>
         <v/>
       </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="94" t="str">
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="91" t="str">
         <f>reference!F26</f>
         <v/>
       </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="115" t="str">
+      <c r="E24" s="91"/>
+      <c r="F24" s="88" t="str">
         <f>IFERROR(SUM(D24*exp_rxns*(1+$D$20)),"")</f>
         <v/>
       </c>
-      <c r="G24" s="115"/>
+      <c r="G24" s="88"/>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
-      <c r="J24" s="116" t="str">
+      <c r="J24" s="92" t="str">
         <f>reference!E64</f>
         <v/>
       </c>
-      <c r="K24" s="116"/>
+      <c r="K24" s="92"/>
       <c r="L24" s="50" t="str">
         <f>reference!F64</f>
         <v/>
@@ -3577,29 +3577,29 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="95" t="str">
+      <c r="A25" s="87" t="str">
         <f>reference!E27</f>
         <v/>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="94" t="str">
+      <c r="B25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="91" t="str">
         <f>reference!F27</f>
         <v/>
       </c>
-      <c r="E25" s="94"/>
-      <c r="F25" s="115" t="str">
+      <c r="E25" s="91"/>
+      <c r="F25" s="88" t="str">
         <f>IFERROR(SUM(D25*exp_rxns*(1+$D$20)),"")</f>
         <v/>
       </c>
-      <c r="G25" s="115"/>
+      <c r="G25" s="88"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
-      <c r="J25" s="116" t="str">
+      <c r="J25" s="92" t="str">
         <f>reference!E65</f>
         <v/>
       </c>
-      <c r="K25" s="116"/>
+      <c r="K25" s="92"/>
       <c r="L25" s="50" t="str">
         <f>reference!F65</f>
         <v/>
@@ -3610,29 +3610,29 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="95" t="str">
+      <c r="A26" s="87" t="str">
         <f>reference!E28</f>
         <v/>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="94" t="str">
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="91" t="str">
         <f>reference!F28</f>
         <v/>
       </c>
-      <c r="E26" s="94"/>
-      <c r="F26" s="115" t="str">
+      <c r="E26" s="91"/>
+      <c r="F26" s="88" t="str">
         <f>IFERROR(SUM(D26*exp_rxns*(1+$D$20)),"")</f>
         <v/>
       </c>
-      <c r="G26" s="115"/>
+      <c r="G26" s="88"/>
       <c r="H26" s="49"/>
       <c r="I26" s="49"/>
-      <c r="J26" s="116" t="str">
+      <c r="J26" s="92" t="str">
         <f>reference!E66</f>
         <v/>
       </c>
-      <c r="K26" s="116"/>
+      <c r="K26" s="92"/>
       <c r="L26" s="50" t="str">
         <f>reference!F66</f>
         <v/>
@@ -3643,28 +3643,28 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="95" t="str">
+      <c r="A27" s="87" t="str">
         <f>reference!E29</f>
         <v/>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="94" t="str">
+      <c r="B27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="91" t="str">
         <f>reference!F29</f>
         <v/>
       </c>
-      <c r="E27" s="94"/>
-      <c r="F27" s="115" t="str">
+      <c r="E27" s="91"/>
+      <c r="F27" s="88" t="str">
         <f>IFERROR(SUM(D27*exp_rxns*(1+$D$20)),"")</f>
         <v/>
       </c>
-      <c r="G27" s="115"/>
+      <c r="G27" s="88"/>
       <c r="H27" s="8"/>
-      <c r="J27" s="116" t="str">
+      <c r="J27" s="92" t="str">
         <f>reference!E67</f>
         <v/>
       </c>
-      <c r="K27" s="116"/>
+      <c r="K27" s="92"/>
       <c r="L27" s="50" t="str">
         <f>reference!F67</f>
         <v/>
@@ -3675,22 +3675,22 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D28" s="117" t="str">
+      <c r="D28" s="85" t="str">
         <f>IF(SUM(D22:E27)=0,"",SUM(D22:E27))</f>
         <v/>
       </c>
-      <c r="E28" s="117"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="52" t="str">
         <f>CONCATENATE("Add ",SUM(D23:D27)," µl of MM to each well")</f>
         <v>Add 0 µl of MM to each well</v>
       </c>
       <c r="G28" s="50"/>
       <c r="H28" s="8"/>
-      <c r="J28" s="116" t="str">
+      <c r="J28" s="92" t="str">
         <f>reference!E68</f>
         <v/>
       </c>
-      <c r="K28" s="116"/>
+      <c r="K28" s="92"/>
       <c r="L28" s="50" t="str">
         <f>reference!F68</f>
         <v/>
@@ -3709,7 +3709,7 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -3718,28 +3718,28 @@
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
-      <c r="K30" s="118" t="s">
+      <c r="K30" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
     </row>
     <row r="31" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="86" t="s">
-        <v>291</v>
-      </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="86"/>
-      <c r="M31" s="86"/>
+      <c r="A31" s="104" t="s">
+        <v>290</v>
+      </c>
+      <c r="B31" s="104"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="104"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
@@ -3752,11 +3752,11 @@
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="8"/>
-      <c r="K32" s="114" t="s">
+      <c r="K32" s="95" t="s">
         <v>162</v>
       </c>
-      <c r="L32" s="114"/>
-      <c r="M32" s="114"/>
+      <c r="L32" s="95"/>
+      <c r="M32" s="95"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
@@ -3773,13 +3773,13 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4252,17 +4252,51 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="72">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C17:K18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="K32:M32"/>
     <mergeCell ref="D24:E24"/>
@@ -4279,51 +4313,17 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C17:K18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <conditionalFormatting sqref="A25:C27">
     <cfRule type="expression" dxfId="12" priority="9">
@@ -4488,13 +4488,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="57" t="s">
         <v>132</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E2" s="58" t="s">
         <v>5</v>
@@ -7784,13 +7784,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3" s="84" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>143</v>
@@ -7990,13 +7990,13 @@
     </row>
     <row r="23" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F24" s="53" t="str">
         <f>IF(pcr_enzyme=$E$14,F32,IF(pcr_enzyme=$E$15,F42,IF(pcr_enzyme=$E$16,F52,"")))</f>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F32">
         <v>8</v>
@@ -8069,7 +8069,7 @@
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F33">
         <f>SUM(F35:F38)</f>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F34">
         <v>25</v>
@@ -8134,7 +8134,7 @@
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F42">
         <v>8</v>
@@ -8142,7 +8142,7 @@
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F43">
         <f>SUM(F45:F46)</f>
@@ -8151,7 +8151,7 @@
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F44">
         <v>25</v>
@@ -8159,7 +8159,7 @@
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F45">
         <v>15.5</v>
@@ -8200,7 +8200,7 @@
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F52">
         <v>5</v>
@@ -8208,7 +8208,7 @@
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F53">
         <f>SUM(F55:F56)</f>
@@ -8217,7 +8217,7 @@
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F54">
         <v>25</v>
@@ -8375,7 +8375,7 @@
         <v>93</v>
       </c>
       <c r="F71" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G71" s="54"/>
     </row>
@@ -8433,7 +8433,7 @@
         <v>8</v>
       </c>
       <c r="F77" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8448,7 +8448,7 @@
         <v>95</v>
       </c>
       <c r="F79" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="5:7" x14ac:dyDescent="0.25">
@@ -8494,7 +8494,7 @@
         <v>8</v>
       </c>
       <c r="F84" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
@@ -8512,7 +8512,7 @@
         <v>93</v>
       </c>
       <c r="F87" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G87" s="54"/>
     </row>
@@ -8570,7 +8570,7 @@
         <v>8</v>
       </c>
       <c r="F93" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="94" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8585,7 +8585,7 @@
         <v>93</v>
       </c>
       <c r="F95" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G95" s="54"/>
     </row>
@@ -8643,12 +8643,12 @@
         <v>8</v>
       </c>
       <c r="F101" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E103" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.25">
@@ -8900,7 +8900,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8951,7 +8951,7 @@
         <v>175</v>
       </c>
       <c r="M1" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="N1" t="s">
         <v>213</v>
@@ -9016,7 +9016,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vph7DaMh3SyowaNNd8/hWiOan38yUHTDW1w5tTlbGEdRpJuRTmeOvrHT9rmEAjHGl0Numj/KRrc+UvQhk/Kdtg==" saltValue="/M7Z5DLigzvvgEv+lbbvig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="V+On3mIKG4iDZA8VJY6RI0Q6K2t5nPFCHUFDR5Wf2KezEa6AP2JR8g95oyax6L0T57Vz84OCXrdSZwmrPTXHGw==" saltValue="2SO4eaxQv1qdVdrK8GKI/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>